<commit_message>
在server.model/demo 文件夹下创建 一个Account 目录 编写Account类 在server.hotfix/demo 文件夹下打开factory类，里面的Create方法 zai sceneTYpe中添加Account类型 在server.hotfix/demo文件夹下创建Account文件夹，创建接收的类 打开client unity.hotfix下面的codes/hotfix/demo/login/loginhelper 修改Login方法 创建登录session 在client unity.model 下面 codes/model/demo/下面创建Account 添加AccountInfoComponent组件类继承ENtity Iawake，idestroy类等
</commit_message>
<xml_diff>
--- a/Excel/StartSceneConfig@s.xlsx
+++ b/Excel/StartSceneConfig@s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13500"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="StartSceneConfig" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Map2</t>
+  </si>
+  <si>
+    <t>Account</t>
   </si>
   <si>
     <t>Robot</t>
@@ -91,10 +94,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -118,21 +121,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -141,22 +129,75 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,52 +212,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -224,15 +219,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,30 +237,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,43 +287,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,139 +443,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,21 +478,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -504,15 +492,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,20 +513,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,151 +543,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1086,10 +1089,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:H11"/>
+  <dimension ref="C3:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1275,6 +1278,26 @@
         <v>20</v>
       </c>
       <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="3:8">
+      <c r="C12" s="3">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3">
+        <v>10005</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1373,10 +1396,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" s="5"/>
     </row>

</xml_diff>